<commit_message>
Added images to breed_data
</commit_message>
<xml_diff>
--- a/seed_data/breed_data.xlsx
+++ b/seed_data/breed_data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="18760" yWindow="460" windowWidth="17040" windowHeight="20440" tabRatio="500"/>
+    <workbookView xWindow="12560" yWindow="500" windowWidth="21040" windowHeight="20440" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1590" uniqueCount="830">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1857" uniqueCount="1097">
   <si>
     <t>BREED_NAME</t>
   </si>
@@ -2524,19 +2524,825 @@
   </si>
   <si>
     <t>http://www.akc.org/dog-breeds/st-bernard</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/affenpischer094_thumb_2.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/afghanThumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/airedaleThumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/Akita_thumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/alaskanMalamuteThumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/AmericanEnglishCoonhound_thumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/AmerEskimoThumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/AmericanFoxhound_thumb_2.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/AmericanHairlessTerrier_thumb_2.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/AmericanLeopardHound_thumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/amStaffTerThumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/AmericanWaterSpanThumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/AnatolianShepherdDog_thumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/AppenzellerSennenhunde_thumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/auscattledogThumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/ausShepherdThumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/australianTerThumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/azawakh.jpg</t>
+  </si>
+  <si>
+    <t>http://cdn.akc.org/akcdoglovers/airedaleThumb.jpg</t>
+  </si>
+  <si>
+    <t>http://cdn.akc.org/akcdoglovers/Akita_thumb.jpg</t>
+  </si>
+  <si>
+    <t>http://cdn.akc.org/akcdoglovers/alaskanMalamuteThumb.jpg</t>
+  </si>
+  <si>
+    <t>http://cdn.akc.org/akcdoglovers/AmericanEnglishCoonhound_thumb.jpg</t>
+  </si>
+  <si>
+    <t>http://cdn.akc.org/AmerEskimoThumb.jpg</t>
+  </si>
+  <si>
+    <t>http://cdn.akc.org/akcdoglovers/AmericanFoxhound_thumb_2.jpg</t>
+  </si>
+  <si>
+    <t>http://cdn.akc.org/akcdoglovers/AmericanHairlessTerrier_thumb_2.jpg</t>
+  </si>
+  <si>
+    <t>http://cdn.akc.org/akcdoglovers/AmericanLeopardHound_thumb.jpg</t>
+  </si>
+  <si>
+    <t>http://cdn.akc.org/akcdoglovers/amStaffTerThumb.jpg</t>
+  </si>
+  <si>
+    <t>http://cdn.akc.org/AmericanWaterSpanThumb.jpg</t>
+  </si>
+  <si>
+    <t>http://cdn.akc.org/akcdoglovers/AnatolianShepherdDog_thumb.jpg</t>
+  </si>
+  <si>
+    <t>http://cdn.akc.org/akcdoglovers/AppenzellerSennenhunde_thumb.jpg</t>
+  </si>
+  <si>
+    <t>http://cdn.akc.org/auscattledogThumb.jpg</t>
+  </si>
+  <si>
+    <t>http://cdn.akc.org/ausShepherdThumb.jpg</t>
+  </si>
+  <si>
+    <t>http://cdn.akc.org/akcdoglovers/australianTerThumb.jpg</t>
+  </si>
+  <si>
+    <t>http://cdn.akc.org/akcdoglovers/azawakh.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/Barbet_thumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/basenjiThumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/Basset-Fauve-De-Bretagne_163X140.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/Basset-Hound_163X140.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/beagleThumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/beardieThumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/Beauceron_163X140.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/bedlingtonTerThumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/Belgian-Laekenois_163X140.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/belgmalinoisThumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/belgsheepdogThumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/belgtervThumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/lg_bergamasco2.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/lg_berger_picard12.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/berneseMountainDogThumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/BichonFriseThumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/BiewerTerrier_thumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/BlackandTanThumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/Black-Russian-Terrier_163X140.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/bloodhoundThumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/Bluetick-Coonhound_163X140.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/Boerboel_thumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/Bolognese_thumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/bordercollieThumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/borderTerThumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/borzoiThumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/bostonTerThumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/bouvierThumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/boxerThumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/BoykinSpaniel_thumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/BraccoItaliano_thumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/BraqueDuBourbonnais_thumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akccontentimages/DSC00658.JPG</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/briardThumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/brittanyThumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/Broholmer_163X140.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/brusselsGriffonThumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/bullTerThumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/bulldogThumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/bullmastiffThumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/cairnTerThumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/CaneCorso_163X140.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/cardiganwelshcorgiThumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/CatahoulaLeopardDog_thumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/CaucasianOvcharka_thumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/CavalierKingCharlesThumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/CentralAsianShepherdDog_thumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/Cesky_thumbNew.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/ChesapeakeBayRetThumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/chihuahuaSmoothThumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/chineseCrestedThumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/chineseSharPei_163X140.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/Chinook_thumbNew.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/chowChowThumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/Cirneco-Dell-Etna_163X140.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/clumberThumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/cockerThumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/collie_thumb_2.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/Coton_thumbNew.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/curlyCoatedRetThumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/CzechoslovakianVlcak_thumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/Dachshund_thumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/dalmatianThumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/dandieDinmontThumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/DanishSwedishFarmdog_thumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/Deutscher-Wachtelhund_163X140.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/dobermanThumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/lg_argentine_dogo15.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/DogueDeBordeauxThumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/DrentschePatrijshond_thumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akccontentimages/Breeds/Drever/drever_thumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/DutchShepherd_thumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/EnglishCockerThumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/EngFoxhoundThumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/EnglishSetterThumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/EngSpringerSpanThumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/EnglishToySpanThumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/EntlebucherMountainDog_thumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/EstrelaMountainDog_163X140.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/Eurasier_163X140.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/finnishSpitzThumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/FlatCoatedRetThumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/frenchieThumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/french-spaniel_163X140.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/GermanLonghairedPointer_thumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/germanPinscherThumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/German-Shepherd-Dog_163X140.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/German-Shorthaired-Pointer_163X140.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/GermanSpitz_thumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/GermanWirehPointThumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/giantSchnauzerThumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/GlenofImaalThumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/GoldenRetThumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/GordonSetThumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/gbgv2.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/greatDaneThumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/greatPyreneesThumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/greaterSwissMountainDogThumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/Greyhound_thumb_2.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/Hamiltonstovare_thumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/harrierThumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/HavaneseThumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/Breeds/Hokkaido/HokkaidoRed2.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/Hovawart_thumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/IbizanThumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/IcelandicSheepdog_thumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/IrishRedandWhiteSetter_thumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/IrishSetThumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/irishTerThumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/IrishWaterSpanThumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/IrishWolfhoundThumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/italianGreyhoundThumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/Jagdterrier_thumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/japaneseChinThumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/KaiKen_thumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/KarelianBearDog_thumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/Keeshond_163X140.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/kerryBlueThumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/KishuKen_thumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/komondorThumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/Kromfohrlander_thumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/kuvaszThumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/LabradorRetThumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/lagotto_romagnolo.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/lakelandTerThumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/LancashireHeeler_thumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/Leo_thumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/llasaApsoThumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/lowchenThumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/malteseThumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/manchesterTerThumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/mastiffThumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/Miniature_American_Shepherd_thumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/miniBullTerThumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/minpinThumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/miniatureSchnauzerThumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/Mudi_thumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/NeoMastiffThumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/Nederlandse-Kooikerhondje_163X140.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/newfoundlandThumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/norfolkThumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/Norrbottenspets_thumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/NorwegianBuhund_thumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/NorElkhoundThumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/Norwegian-Lundehund_163X140.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/Norwich_Terrier_163X140.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/NovaScotiaDuckTollingRetriever_thumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/oldengsheepThumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/otterhoundThumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/papillonThumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/parsonRussellThumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/pekingeseThumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/pembrokewelshcorgiThumb-1.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/PerroDePresaCanario_thumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/peruvian_inca_orchid.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/pbgvThumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/pharoahHoundThumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/plotthoundThumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/PointerThumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/PolishLSThumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/pomeranianThumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/ToyPoodleThumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/portuguese_podengo.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/PortuguesePodengoPequeno_thumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/breedthumbs/PortuguesePointer_thumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/PortugueseSheepdog_thumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/portugueseWaterDogThumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/pugThumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/puliThumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/pumi.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/PyreneanMastiff_163X140.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/PyreneanShepherd_thumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/RafeiroDoAlentejo_thumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/RatTerrier_thumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/redboneThumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/rRidgebackThumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/rottweilerThumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/RussellTerrier_thumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/RussianToy_thumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akccontentimages/Breeds/Russian_Tsvetnaya_Bolonka/Russian_Tsvetnaya_Bolonka_thumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/salukiThumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/SamoyedThumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/Schapendoes_thumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/schipperkeThumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/ScottishDeerhound_163X140.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/scottyThumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/sealyhamTerThumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/ShetlandSheepdog_thumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/shibaInuThumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/shihTzuThumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/ShikokuThumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/SiberianHuskyThumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/silkyTerThumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/SkyeTerThumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/sloughi.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/SlovenskyCuvac_thumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/breedthumbs/adult_male_slovensky_kopov_1.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/breedthumbs/SmallMunsterlanderPointer_thumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/smoothFoxTerThumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/Soft-Coated-Wheaten-Terrier_163X140.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/SpanishMastiff_163X140.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/SpanishWaterDogcropped.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/SpinoneThumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/StBernardThumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/Stabyhoun_thumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/Staffordshire-Bull-Terrier_163X140.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/Standard-Schnauzer_163X140.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/SussexThumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/SwedishLapphund_thumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/swedishVallhundThumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akccontentimages/TRT2.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/ThaiRidgeback_thumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/TibMastiffThumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/TibSpanielThumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/TibTerrierThumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/Tornjak_thumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/Tosa_thumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/toyFoxTerThumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/Transylvanian_Hound_163X140.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/TreeingTennesseeBrindle_thumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/TreeingWalkerCoonhound_thumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/VizslaThumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/weimeranerThumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/WelshSpringerSpanThumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/welshTerThumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/westieThumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/whippet_163X140.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/WireFoxTerThumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/wirePointGriffonThumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/WirehairedVizsla_163X140.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/WorkingKelpie_163X140.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/Xoloitzcuintli_thumb.jpg</t>
+  </si>
+  <si>
+    <t>//cdn.akc.org/akcdoglovers/YorkieThumb.jpg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FFD6D6D6"/>
+      <name val="Menlo"/>
     </font>
   </fonts>
   <fills count="2">
@@ -2559,9 +3365,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2855,10 +3662,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G257"/>
+  <dimension ref="A1:I257"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="F220" workbookViewId="0">
+      <selection activeCell="I258" sqref="I258"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2871,7 +3678,7 @@
     <col min="7" max="7" width="56.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2894,7 +3701,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -2916,8 +3723,11 @@
       <c r="G2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I2" s="2" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -2939,8 +3749,11 @@
       <c r="G3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I3" s="2" t="s">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -2959,8 +3772,14 @@
       <c r="F4" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G4" t="s">
+        <v>848</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>832</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -2979,8 +3798,14 @@
       <c r="F5" t="s">
         <v>632</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G5" t="s">
+        <v>849</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>833</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -2999,8 +3824,14 @@
       <c r="F6" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G6" t="s">
+        <v>850</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>28</v>
       </c>
@@ -3019,8 +3850,14 @@
       <c r="F7" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G7" t="s">
+        <v>851</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>835</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>31</v>
       </c>
@@ -3039,8 +3876,14 @@
       <c r="F8" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G8" t="s">
+        <v>852</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>836</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>35</v>
       </c>
@@ -3059,8 +3902,14 @@
       <c r="F9" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G9" t="s">
+        <v>853</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>837</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>38</v>
       </c>
@@ -3079,8 +3928,14 @@
       <c r="F10" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G10" t="s">
+        <v>854</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>41</v>
       </c>
@@ -3099,8 +3954,14 @@
       <c r="F11" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G11" t="s">
+        <v>855</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>839</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>45</v>
       </c>
@@ -3119,8 +3980,14 @@
       <c r="F12" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G12" t="s">
+        <v>856</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>840</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>48</v>
       </c>
@@ -3139,8 +4006,14 @@
       <c r="F13" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G13" t="s">
+        <v>857</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>52</v>
       </c>
@@ -3159,8 +4032,14 @@
       <c r="F14" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G14" t="s">
+        <v>858</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>842</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>55</v>
       </c>
@@ -3179,8 +4058,14 @@
       <c r="F15" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G15" t="s">
+        <v>859</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>57</v>
       </c>
@@ -3199,8 +4084,14 @@
       <c r="F16" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G16" t="s">
+        <v>860</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>844</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>60</v>
       </c>
@@ -3219,8 +4110,14 @@
       <c r="F17" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G17" t="s">
+        <v>861</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>845</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>62</v>
       </c>
@@ -3239,8 +4136,14 @@
       <c r="F18" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G18" t="s">
+        <v>862</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>846</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>64</v>
       </c>
@@ -3259,8 +4162,14 @@
       <c r="F19" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G19" t="s">
+        <v>863</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>66</v>
       </c>
@@ -3279,8 +4188,11 @@
       <c r="F20" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I20" s="2" t="s">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>68</v>
       </c>
@@ -3299,8 +4211,11 @@
       <c r="F21" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I21" s="2" t="s">
+        <v>865</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>70</v>
       </c>
@@ -3319,8 +4234,11 @@
       <c r="F22" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I22" s="2" t="s">
+        <v>866</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>72</v>
       </c>
@@ -3339,8 +4257,11 @@
       <c r="F23" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I23" s="2" t="s">
+        <v>867</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>74</v>
       </c>
@@ -3359,8 +4280,11 @@
       <c r="F24" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I24" s="2" t="s">
+        <v>868</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>76</v>
       </c>
@@ -3379,8 +4303,11 @@
       <c r="F25" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I25" s="2" t="s">
+        <v>869</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>78</v>
       </c>
@@ -3399,8 +4326,11 @@
       <c r="F26" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I26" s="2" t="s">
+        <v>870</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>80</v>
       </c>
@@ -3419,8 +4349,11 @@
       <c r="F27" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I27" s="2" t="s">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>82</v>
       </c>
@@ -3439,8 +4372,11 @@
       <c r="F28" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I28" s="2" t="s">
+        <v>872</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>84</v>
       </c>
@@ -3459,8 +4395,11 @@
       <c r="F29" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I29" s="2" t="s">
+        <v>873</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>86</v>
       </c>
@@ -3479,8 +4418,11 @@
       <c r="F30" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I30" s="2" t="s">
+        <v>874</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>88</v>
       </c>
@@ -3499,8 +4441,11 @@
       <c r="F31" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I31" s="2" t="s">
+        <v>875</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>90</v>
       </c>
@@ -3519,8 +4464,11 @@
       <c r="F32" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I32" s="2" t="s">
+        <v>876</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>92</v>
       </c>
@@ -3539,8 +4487,11 @@
       <c r="F33" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I33" s="2" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>94</v>
       </c>
@@ -3562,8 +4513,11 @@
       <c r="G34" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I34" s="2" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>98</v>
       </c>
@@ -3582,8 +4536,11 @@
       <c r="F35" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I35" s="2" t="s">
+        <v>879</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>100</v>
       </c>
@@ -3602,8 +4559,11 @@
       <c r="F36" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I36" s="2" t="s">
+        <v>880</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>102</v>
       </c>
@@ -3622,8 +4582,11 @@
       <c r="F37" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I37" s="2" t="s">
+        <v>881</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>104</v>
       </c>
@@ -3645,8 +4608,11 @@
       <c r="G38" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I38" s="2" t="s">
+        <v>882</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>108</v>
       </c>
@@ -3665,8 +4631,11 @@
       <c r="F39" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I39" s="2" t="s">
+        <v>883</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>110</v>
       </c>
@@ -3685,8 +4654,11 @@
       <c r="F40" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I40" s="2" t="s">
+        <v>884</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>112</v>
       </c>
@@ -3705,8 +4677,11 @@
       <c r="F41" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I41" s="2" t="s">
+        <v>885</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>114</v>
       </c>
@@ -3725,8 +4700,11 @@
       <c r="F42" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I42" s="2" t="s">
+        <v>886</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>116</v>
       </c>
@@ -3745,8 +4723,11 @@
       <c r="F43" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I43" s="2" t="s">
+        <v>887</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>118</v>
       </c>
@@ -3765,8 +4746,11 @@
       <c r="F44" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I44" s="2" t="s">
+        <v>888</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>120</v>
       </c>
@@ -3785,8 +4769,11 @@
       <c r="F45" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I45" s="2" t="s">
+        <v>889</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>122</v>
       </c>
@@ -3805,8 +4792,11 @@
       <c r="F46" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I46" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>124</v>
       </c>
@@ -3825,8 +4815,11 @@
       <c r="F47" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I47" s="2" t="s">
+        <v>891</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>126</v>
       </c>
@@ -3845,8 +4838,11 @@
       <c r="F48" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I48" s="2" t="s">
+        <v>892</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>128</v>
       </c>
@@ -3865,8 +4861,11 @@
       <c r="F49" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I49" s="2" t="s">
+        <v>893</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>130</v>
       </c>
@@ -3885,8 +4884,11 @@
       <c r="F50" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I50" s="2" t="s">
+        <v>894</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>132</v>
       </c>
@@ -3905,8 +4907,11 @@
       <c r="F51" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I51" s="2" t="s">
+        <v>895</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>134</v>
       </c>
@@ -3925,8 +4930,11 @@
       <c r="F52" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I52" s="2" t="s">
+        <v>896</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>136</v>
       </c>
@@ -3945,8 +4953,11 @@
       <c r="F53" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I53" s="2" t="s">
+        <v>897</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>138</v>
       </c>
@@ -3968,8 +4979,11 @@
       <c r="G54" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I54" s="2" t="s">
+        <v>898</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>143</v>
       </c>
@@ -3988,8 +5002,11 @@
       <c r="F55" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I55" s="2" t="s">
+        <v>899</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>145</v>
       </c>
@@ -4011,8 +5028,11 @@
       <c r="G56" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I56" s="2" t="s">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>149</v>
       </c>
@@ -4031,8 +5051,11 @@
       <c r="F57" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I57" s="2" t="s">
+        <v>901</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>151</v>
       </c>
@@ -4054,8 +5077,11 @@
       <c r="G58" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I58" s="2" t="s">
+        <v>902</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>155</v>
       </c>
@@ -4077,8 +5103,11 @@
       <c r="G59" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I59" s="2" t="s">
+        <v>903</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>159</v>
       </c>
@@ -4097,8 +5126,11 @@
       <c r="F60" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I60" s="2" t="s">
+        <v>904</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>161</v>
       </c>
@@ -4118,7 +5150,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>163</v>
       </c>
@@ -4140,8 +5172,11 @@
       <c r="G62" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I62" s="2" t="s">
+        <v>905</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>167</v>
       </c>
@@ -4160,8 +5195,11 @@
       <c r="F63" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I63" s="2" t="s">
+        <v>906</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>169</v>
       </c>
@@ -4180,8 +5218,11 @@
       <c r="F64" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I64" s="2" t="s">
+        <v>907</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>171</v>
       </c>
@@ -4200,8 +5241,11 @@
       <c r="F65" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I65" s="2" t="s">
+        <v>908</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>173</v>
       </c>
@@ -4223,8 +5267,11 @@
       <c r="G66" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I66" s="2" t="s">
+        <v>909</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>177</v>
       </c>
@@ -4243,8 +5290,11 @@
       <c r="F67" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I67" s="2" t="s">
+        <v>910</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>179</v>
       </c>
@@ -4263,8 +5313,11 @@
       <c r="F68" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I68" s="2" t="s">
+        <v>911</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>181</v>
       </c>
@@ -4283,8 +5336,11 @@
       <c r="F69" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I69" s="2" t="s">
+        <v>912</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>183</v>
       </c>
@@ -4306,8 +5362,11 @@
       <c r="G70" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I70" s="2" t="s">
+        <v>913</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>187</v>
       </c>
@@ -4329,8 +5388,11 @@
       <c r="G71" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I71" s="2" t="s">
+        <v>914</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>191</v>
       </c>
@@ -4349,8 +5411,11 @@
       <c r="F72" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I72" s="2" t="s">
+        <v>915</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>193</v>
       </c>
@@ -4369,8 +5434,11 @@
       <c r="F73" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I73" s="2" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>195</v>
       </c>
@@ -4389,8 +5457,11 @@
       <c r="F74" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I74" s="2" t="s">
+        <v>917</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>197</v>
       </c>
@@ -4409,8 +5480,11 @@
       <c r="F75" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I75" s="2" t="s">
+        <v>918</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>199</v>
       </c>
@@ -4429,8 +5503,11 @@
       <c r="F76" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I76" s="2" t="s">
+        <v>919</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>201</v>
       </c>
@@ -4452,8 +5529,11 @@
       <c r="G77" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I77" s="2" t="s">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>205</v>
       </c>
@@ -4472,8 +5552,11 @@
       <c r="F78" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I78" s="2" t="s">
+        <v>921</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>207</v>
       </c>
@@ -4492,8 +5575,11 @@
       <c r="F79" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I79" s="2" t="s">
+        <v>922</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>209</v>
       </c>
@@ -4512,8 +5598,11 @@
       <c r="F80" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I80" s="2" t="s">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>211</v>
       </c>
@@ -4532,8 +5621,11 @@
       <c r="F81" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I81" s="2" t="s">
+        <v>924</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>213</v>
       </c>
@@ -4555,8 +5647,11 @@
       <c r="G82" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I82" s="2" t="s">
+        <v>925</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>217</v>
       </c>
@@ -4575,8 +5670,11 @@
       <c r="F83" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I83" s="2" t="s">
+        <v>926</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>219</v>
       </c>
@@ -4595,8 +5693,11 @@
       <c r="F84" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I84" s="2" t="s">
+        <v>927</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>221</v>
       </c>
@@ -4615,8 +5716,11 @@
       <c r="F85" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I85" s="2" t="s">
+        <v>928</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>223</v>
       </c>
@@ -4635,8 +5739,11 @@
       <c r="F86" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I86" s="2" t="s">
+        <v>929</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>225</v>
       </c>
@@ -4655,8 +5762,11 @@
       <c r="F87" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I87" s="2" t="s">
+        <v>930</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>227</v>
       </c>
@@ -4675,8 +5785,11 @@
       <c r="F88" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I88" s="2" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>229</v>
       </c>
@@ -4698,8 +5811,11 @@
       <c r="G89" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I89" s="2" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>233</v>
       </c>
@@ -4718,8 +5834,11 @@
       <c r="F90" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I90" s="2" t="s">
+        <v>933</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>235</v>
       </c>
@@ -4738,8 +5857,11 @@
       <c r="F91" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I91" s="2" t="s">
+        <v>934</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>237</v>
       </c>
@@ -4758,8 +5880,11 @@
       <c r="F92" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I92" s="2" t="s">
+        <v>935</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>239</v>
       </c>
@@ -4778,8 +5903,11 @@
       <c r="F93" t="s">
         <v>240</v>
       </c>
-    </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I93" s="2" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>241</v>
       </c>
@@ -4798,8 +5926,11 @@
       <c r="F94" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I94" s="2" t="s">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>243</v>
       </c>
@@ -4818,8 +5949,11 @@
       <c r="F95" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I95" s="2" t="s">
+        <v>938</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>245</v>
       </c>
@@ -4841,8 +5975,11 @@
       <c r="G96" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I96" s="2" t="s">
+        <v>939</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>249</v>
       </c>
@@ -4864,8 +6001,11 @@
       <c r="G97" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I97" s="2" t="s">
+        <v>940</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>253</v>
       </c>
@@ -4884,8 +6024,11 @@
       <c r="F98" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I98" s="2" t="s">
+        <v>941</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>255</v>
       </c>
@@ -4904,8 +6047,11 @@
       <c r="F99" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I99" s="2" t="s">
+        <v>942</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>257</v>
       </c>
@@ -4924,8 +6070,11 @@
       <c r="F100" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I100" s="2" t="s">
+        <v>943</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>259</v>
       </c>
@@ -4944,8 +6093,9 @@
       <c r="F101" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I101" s="2"/>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>261</v>
       </c>
@@ -4965,7 +6115,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>263</v>
       </c>
@@ -4984,8 +6134,11 @@
       <c r="F103" t="s">
         <v>264</v>
       </c>
-    </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I103" s="2" t="s">
+        <v>944</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>265</v>
       </c>
@@ -5004,8 +6157,11 @@
       <c r="F104" t="s">
         <v>266</v>
       </c>
-    </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I104" s="2" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>267</v>
       </c>
@@ -5024,8 +6180,11 @@
       <c r="F105" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I105" s="2" t="s">
+        <v>946</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>269</v>
       </c>
@@ -5044,8 +6203,11 @@
       <c r="F106" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I106" s="2" t="s">
+        <v>947</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>271</v>
       </c>
@@ -5064,8 +6226,11 @@
       <c r="F107" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I107" s="2" t="s">
+        <v>948</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>273</v>
       </c>
@@ -5084,8 +6249,11 @@
       <c r="F108" t="s">
         <v>274</v>
       </c>
-    </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I108" s="2" t="s">
+        <v>949</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>275</v>
       </c>
@@ -5104,8 +6272,11 @@
       <c r="F109" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I109" s="2" t="s">
+        <v>950</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>277</v>
       </c>
@@ -5124,8 +6295,11 @@
       <c r="F110" t="s">
         <v>278</v>
       </c>
-    </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I110" s="2" t="s">
+        <v>951</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>279</v>
       </c>
@@ -5144,8 +6318,11 @@
       <c r="F111" t="s">
         <v>280</v>
       </c>
-    </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I111" s="2" t="s">
+        <v>952</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>281</v>
       </c>
@@ -5164,8 +6341,11 @@
       <c r="F112" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I112" s="2" t="s">
+        <v>953</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>283</v>
       </c>
@@ -5184,8 +6364,11 @@
       <c r="F113" t="s">
         <v>284</v>
       </c>
-    </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I113" s="2" t="s">
+        <v>954</v>
+      </c>
+    </row>
+    <row r="114" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>285</v>
       </c>
@@ -5204,8 +6387,11 @@
       <c r="F114" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I114" s="2" t="s">
+        <v>955</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>287</v>
       </c>
@@ -5224,8 +6410,11 @@
       <c r="F115" t="s">
         <v>288</v>
       </c>
-    </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I115" s="2" t="s">
+        <v>956</v>
+      </c>
+    </row>
+    <row r="116" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>289</v>
       </c>
@@ -5244,8 +6433,11 @@
       <c r="F116" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I116" s="2" t="s">
+        <v>957</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>291</v>
       </c>
@@ -5264,8 +6456,11 @@
       <c r="F117" t="s">
         <v>292</v>
       </c>
-    </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I117" s="2" t="s">
+        <v>958</v>
+      </c>
+    </row>
+    <row r="118" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>293</v>
       </c>
@@ -5287,8 +6482,11 @@
       <c r="G118" t="s">
         <v>296</v>
       </c>
-    </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I118" s="2" t="s">
+        <v>959</v>
+      </c>
+    </row>
+    <row r="119" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>297</v>
       </c>
@@ -5310,8 +6508,11 @@
       <c r="G119" t="s">
         <v>300</v>
       </c>
-    </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I119" s="2" t="s">
+        <v>960</v>
+      </c>
+    </row>
+    <row r="120" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>301</v>
       </c>
@@ -5330,8 +6531,11 @@
       <c r="F120" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I120" s="2" t="s">
+        <v>961</v>
+      </c>
+    </row>
+    <row r="121" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>303</v>
       </c>
@@ -5350,8 +6554,11 @@
       <c r="F121" t="s">
         <v>304</v>
       </c>
-    </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I121" s="2" t="s">
+        <v>962</v>
+      </c>
+    </row>
+    <row r="122" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>305</v>
       </c>
@@ -5370,8 +6577,11 @@
       <c r="F122" t="s">
         <v>306</v>
       </c>
-    </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I122" s="2" t="s">
+        <v>963</v>
+      </c>
+    </row>
+    <row r="123" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>307</v>
       </c>
@@ -5390,8 +6600,11 @@
       <c r="F123" t="s">
         <v>308</v>
       </c>
-    </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I123" s="2" t="s">
+        <v>964</v>
+      </c>
+    </row>
+    <row r="124" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>309</v>
       </c>
@@ -5413,8 +6626,11 @@
       <c r="G124" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I124" s="2" t="s">
+        <v>965</v>
+      </c>
+    </row>
+    <row r="125" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>313</v>
       </c>
@@ -5433,8 +6649,11 @@
       <c r="F125" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I125" s="2" t="s">
+        <v>966</v>
+      </c>
+    </row>
+    <row r="126" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>315</v>
       </c>
@@ -5453,8 +6672,11 @@
       <c r="F126" t="s">
         <v>316</v>
       </c>
-    </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I126" s="2" t="s">
+        <v>967</v>
+      </c>
+    </row>
+    <row r="127" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>317</v>
       </c>
@@ -5473,8 +6695,11 @@
       <c r="F127" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I127" s="2" t="s">
+        <v>968</v>
+      </c>
+    </row>
+    <row r="128" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>319</v>
       </c>
@@ -5493,8 +6718,11 @@
       <c r="F128" t="s">
         <v>320</v>
       </c>
-    </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I128" s="2" t="s">
+        <v>969</v>
+      </c>
+    </row>
+    <row r="129" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>321</v>
       </c>
@@ -5513,8 +6741,11 @@
       <c r="F129" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I129" s="2" t="s">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="130" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>323</v>
       </c>
@@ -5533,8 +6764,11 @@
       <c r="F130" t="s">
         <v>324</v>
       </c>
-    </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I130" s="2" t="s">
+        <v>971</v>
+      </c>
+    </row>
+    <row r="131" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>325</v>
       </c>
@@ -5553,8 +6787,11 @@
       <c r="F131" t="s">
         <v>326</v>
       </c>
-    </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I131" s="2" t="s">
+        <v>972</v>
+      </c>
+    </row>
+    <row r="132" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>327</v>
       </c>
@@ -5573,8 +6810,11 @@
       <c r="F132" t="s">
         <v>328</v>
       </c>
-    </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I132" s="2" t="s">
+        <v>973</v>
+      </c>
+    </row>
+    <row r="133" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>329</v>
       </c>
@@ -5596,8 +6836,11 @@
       <c r="G133" t="s">
         <v>332</v>
       </c>
-    </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I133" s="2" t="s">
+        <v>974</v>
+      </c>
+    </row>
+    <row r="134" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>333</v>
       </c>
@@ -5619,8 +6862,11 @@
       <c r="G134" t="s">
         <v>336</v>
       </c>
-    </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I134" s="2" t="s">
+        <v>975</v>
+      </c>
+    </row>
+    <row r="135" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>337</v>
       </c>
@@ -5639,8 +6885,11 @@
       <c r="F135" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I135" s="2" t="s">
+        <v>976</v>
+      </c>
+    </row>
+    <row r="136" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>339</v>
       </c>
@@ -5662,8 +6911,11 @@
       <c r="G136" t="s">
         <v>342</v>
       </c>
-    </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I136" s="2" t="s">
+        <v>977</v>
+      </c>
+    </row>
+    <row r="137" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>343</v>
       </c>
@@ -5682,8 +6934,9 @@
       <c r="F137" t="s">
         <v>344</v>
       </c>
-    </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I137" s="2"/>
+    </row>
+    <row r="138" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>345</v>
       </c>
@@ -5702,8 +6955,11 @@
       <c r="F138" t="s">
         <v>346</v>
       </c>
-    </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I138" s="2" t="s">
+        <v>978</v>
+      </c>
+    </row>
+    <row r="139" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>347</v>
       </c>
@@ -5722,8 +6978,11 @@
       <c r="F139" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I139" s="2" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="140" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>349</v>
       </c>
@@ -5742,8 +7001,11 @@
       <c r="F140" t="s">
         <v>350</v>
       </c>
-    </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I140" s="2" t="s">
+        <v>980</v>
+      </c>
+    </row>
+    <row r="141" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>351</v>
       </c>
@@ -5762,8 +7024,11 @@
       <c r="F141" t="s">
         <v>352</v>
       </c>
-    </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I141" s="2" t="s">
+        <v>981</v>
+      </c>
+    </row>
+    <row r="142" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>353</v>
       </c>
@@ -5782,8 +7047,11 @@
       <c r="F142" t="s">
         <v>354</v>
       </c>
-    </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I142" s="2" t="s">
+        <v>982</v>
+      </c>
+    </row>
+    <row r="143" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>355</v>
       </c>
@@ -5802,8 +7070,11 @@
       <c r="F143" t="s">
         <v>356</v>
       </c>
-    </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I143" s="2" t="s">
+        <v>983</v>
+      </c>
+    </row>
+    <row r="144" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>357</v>
       </c>
@@ -5822,8 +7093,11 @@
       <c r="F144" t="s">
         <v>358</v>
       </c>
-    </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I144" s="2" t="s">
+        <v>984</v>
+      </c>
+    </row>
+    <row r="145" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>359</v>
       </c>
@@ -5842,8 +7116,11 @@
       <c r="F145" t="s">
         <v>360</v>
       </c>
-    </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I145" s="2" t="s">
+        <v>985</v>
+      </c>
+    </row>
+    <row r="146" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>361</v>
       </c>
@@ -5862,8 +7139,11 @@
       <c r="F146" t="s">
         <v>362</v>
       </c>
-    </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I146" s="2" t="s">
+        <v>986</v>
+      </c>
+    </row>
+    <row r="147" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>363</v>
       </c>
@@ -5882,8 +7162,11 @@
       <c r="F147" t="s">
         <v>364</v>
       </c>
-    </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I147" s="2" t="s">
+        <v>987</v>
+      </c>
+    </row>
+    <row r="148" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>365</v>
       </c>
@@ -5902,8 +7185,11 @@
       <c r="F148" t="s">
         <v>366</v>
       </c>
-    </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I148" s="2" t="s">
+        <v>988</v>
+      </c>
+    </row>
+    <row r="149" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>367</v>
       </c>
@@ -5922,8 +7208,11 @@
       <c r="F149" t="s">
         <v>368</v>
       </c>
-    </row>
-    <row r="150" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I149" s="2" t="s">
+        <v>989</v>
+      </c>
+    </row>
+    <row r="150" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>369</v>
       </c>
@@ -5945,8 +7234,11 @@
       <c r="G150" t="s">
         <v>372</v>
       </c>
-    </row>
-    <row r="151" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I150" s="2" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="151" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>373</v>
       </c>
@@ -5965,8 +7257,11 @@
       <c r="F151" t="s">
         <v>374</v>
       </c>
-    </row>
-    <row r="152" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I151" s="2" t="s">
+        <v>991</v>
+      </c>
+    </row>
+    <row r="152" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>375</v>
       </c>
@@ -5985,8 +7280,11 @@
       <c r="F152" t="s">
         <v>376</v>
       </c>
-    </row>
-    <row r="153" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I152" s="2" t="s">
+        <v>992</v>
+      </c>
+    </row>
+    <row r="153" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>377</v>
       </c>
@@ -6008,8 +7306,11 @@
       <c r="G153" t="s">
         <v>380</v>
       </c>
-    </row>
-    <row r="154" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I153" s="2" t="s">
+        <v>993</v>
+      </c>
+    </row>
+    <row r="154" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>381</v>
       </c>
@@ -6031,8 +7332,11 @@
       <c r="G154" t="s">
         <v>384</v>
       </c>
-    </row>
-    <row r="155" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I154" s="2" t="s">
+        <v>994</v>
+      </c>
+    </row>
+    <row r="155" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>385</v>
       </c>
@@ -6054,8 +7358,11 @@
       <c r="G155" t="s">
         <v>388</v>
       </c>
-    </row>
-    <row r="156" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I155" s="2" t="s">
+        <v>995</v>
+      </c>
+    </row>
+    <row r="156" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>389</v>
       </c>
@@ -6074,8 +7381,11 @@
       <c r="F156" t="s">
         <v>390</v>
       </c>
-    </row>
-    <row r="157" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I156" s="2" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="157" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>391</v>
       </c>
@@ -6094,8 +7404,11 @@
       <c r="F157" t="s">
         <v>392</v>
       </c>
-    </row>
-    <row r="158" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I157" s="2" t="s">
+        <v>997</v>
+      </c>
+    </row>
+    <row r="158" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>393</v>
       </c>
@@ -6117,8 +7430,11 @@
       <c r="G158" t="s">
         <v>396</v>
       </c>
-    </row>
-    <row r="159" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I158" s="2" t="s">
+        <v>998</v>
+      </c>
+    </row>
+    <row r="159" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>397</v>
       </c>
@@ -6137,8 +7453,11 @@
       <c r="F159" t="s">
         <v>398</v>
       </c>
-    </row>
-    <row r="160" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I159" s="2" t="s">
+        <v>999</v>
+      </c>
+    </row>
+    <row r="160" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>399</v>
       </c>
@@ -6157,8 +7476,11 @@
       <c r="F160" t="s">
         <v>400</v>
       </c>
-    </row>
-    <row r="161" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I160" s="2" t="s">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="161" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>401</v>
       </c>
@@ -6180,8 +7502,11 @@
       <c r="G161" t="s">
         <v>404</v>
       </c>
-    </row>
-    <row r="162" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I161" s="2" t="s">
+        <v>1001</v>
+      </c>
+    </row>
+    <row r="162" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>405</v>
       </c>
@@ -6200,8 +7525,11 @@
       <c r="F162" t="s">
         <v>406</v>
       </c>
-    </row>
-    <row r="163" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I162" s="2" t="s">
+        <v>1002</v>
+      </c>
+    </row>
+    <row r="163" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>407</v>
       </c>
@@ -6223,8 +7551,11 @@
       <c r="G163" t="s">
         <v>410</v>
       </c>
-    </row>
-    <row r="164" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I163" s="2" t="s">
+        <v>1003</v>
+      </c>
+    </row>
+    <row r="164" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>411</v>
       </c>
@@ -6246,8 +7577,11 @@
       <c r="G164" t="s">
         <v>414</v>
       </c>
-    </row>
-    <row r="165" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I164" s="2" t="s">
+        <v>1004</v>
+      </c>
+    </row>
+    <row r="165" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>415</v>
       </c>
@@ -6266,8 +7600,11 @@
       <c r="F165" t="s">
         <v>416</v>
       </c>
-    </row>
-    <row r="166" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I165" s="2" t="s">
+        <v>1005</v>
+      </c>
+    </row>
+    <row r="166" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>417</v>
       </c>
@@ -6286,8 +7623,11 @@
       <c r="F166" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="167" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I166" s="2" t="s">
+        <v>1006</v>
+      </c>
+    </row>
+    <row r="167" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>419</v>
       </c>
@@ -6306,8 +7646,11 @@
       <c r="F167" t="s">
         <v>420</v>
       </c>
-    </row>
-    <row r="168" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I167" s="2" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="168" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>421</v>
       </c>
@@ -6326,8 +7669,11 @@
       <c r="F168" t="s">
         <v>422</v>
       </c>
-    </row>
-    <row r="169" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I168" s="2" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="169" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>423</v>
       </c>
@@ -6349,8 +7695,11 @@
       <c r="G169" t="s">
         <v>426</v>
       </c>
-    </row>
-    <row r="170" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I169" s="2" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="170" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>427</v>
       </c>
@@ -6369,8 +7718,11 @@
       <c r="F170" t="s">
         <v>428</v>
       </c>
-    </row>
-    <row r="171" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I170" s="2" t="s">
+        <v>1010</v>
+      </c>
+    </row>
+    <row r="171" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>429</v>
       </c>
@@ -6389,8 +7741,11 @@
       <c r="F171" t="s">
         <v>430</v>
       </c>
-    </row>
-    <row r="172" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I171" s="2" t="s">
+        <v>1011</v>
+      </c>
+    </row>
+    <row r="172" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>431</v>
       </c>
@@ -6409,8 +7764,11 @@
       <c r="F172" t="s">
         <v>432</v>
       </c>
-    </row>
-    <row r="173" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I172" s="2" t="s">
+        <v>1012</v>
+      </c>
+    </row>
+    <row r="173" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>433</v>
       </c>
@@ -6432,8 +7790,11 @@
       <c r="G173" t="s">
         <v>436</v>
       </c>
-    </row>
-    <row r="174" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I173" s="2" t="s">
+        <v>1013</v>
+      </c>
+    </row>
+    <row r="174" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>437</v>
       </c>
@@ -6452,8 +7813,11 @@
       <c r="F174" t="s">
         <v>438</v>
       </c>
-    </row>
-    <row r="175" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I174" s="2" t="s">
+        <v>1014</v>
+      </c>
+    </row>
+    <row r="175" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>439</v>
       </c>
@@ -6475,8 +7839,11 @@
       <c r="G175" t="s">
         <v>442</v>
       </c>
-    </row>
-    <row r="176" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I175" s="2" t="s">
+        <v>1015</v>
+      </c>
+    </row>
+    <row r="176" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>443</v>
       </c>
@@ -6498,8 +7865,11 @@
       <c r="G176" t="s">
         <v>446</v>
       </c>
-    </row>
-    <row r="177" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I176" s="2" t="s">
+        <v>1016</v>
+      </c>
+    </row>
+    <row r="177" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>447</v>
       </c>
@@ -6518,8 +7888,11 @@
       <c r="F177" t="s">
         <v>448</v>
       </c>
-    </row>
-    <row r="178" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I177" s="2" t="s">
+        <v>1017</v>
+      </c>
+    </row>
+    <row r="178" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>449</v>
       </c>
@@ -6538,8 +7911,11 @@
       <c r="F178" t="s">
         <v>450</v>
       </c>
-    </row>
-    <row r="179" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I178" s="2" t="s">
+        <v>1018</v>
+      </c>
+    </row>
+    <row r="179" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>451</v>
       </c>
@@ -6558,8 +7934,11 @@
       <c r="F179" t="s">
         <v>452</v>
       </c>
-    </row>
-    <row r="180" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I179" s="2" t="s">
+        <v>1019</v>
+      </c>
+    </row>
+    <row r="180" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
         <v>453</v>
       </c>
@@ -6578,8 +7957,11 @@
       <c r="F180" t="s">
         <v>454</v>
       </c>
-    </row>
-    <row r="181" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I180" s="2" t="s">
+        <v>1020</v>
+      </c>
+    </row>
+    <row r="181" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>455</v>
       </c>
@@ -6598,8 +7980,11 @@
       <c r="F181" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="182" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I181" s="2" t="s">
+        <v>1021</v>
+      </c>
+    </row>
+    <row r="182" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
         <v>457</v>
       </c>
@@ -6618,8 +8003,11 @@
       <c r="F182" t="s">
         <v>458</v>
       </c>
-    </row>
-    <row r="183" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I182" s="2" t="s">
+        <v>1022</v>
+      </c>
+    </row>
+    <row r="183" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
         <v>459</v>
       </c>
@@ -6638,8 +8026,11 @@
       <c r="F183" t="s">
         <v>460</v>
       </c>
-    </row>
-    <row r="184" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I183" s="2" t="s">
+        <v>1023</v>
+      </c>
+    </row>
+    <row r="184" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
         <v>461</v>
       </c>
@@ -6661,8 +8052,11 @@
       <c r="G184" t="s">
         <v>464</v>
       </c>
-    </row>
-    <row r="185" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I184" s="2" t="s">
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="185" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
         <v>465</v>
       </c>
@@ -6684,8 +8078,11 @@
       <c r="G185" t="s">
         <v>468</v>
       </c>
-    </row>
-    <row r="186" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I185" s="2" t="s">
+        <v>1025</v>
+      </c>
+    </row>
+    <row r="186" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>469</v>
       </c>
@@ -6704,8 +8101,11 @@
       <c r="F186" t="s">
         <v>470</v>
       </c>
-    </row>
-    <row r="187" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I186" s="2" t="s">
+        <v>1026</v>
+      </c>
+    </row>
+    <row r="187" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
         <v>471</v>
       </c>
@@ -6724,8 +8124,11 @@
       <c r="F187" t="s">
         <v>472</v>
       </c>
-    </row>
-    <row r="188" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I187" s="2" t="s">
+        <v>1027</v>
+      </c>
+    </row>
+    <row r="188" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>473</v>
       </c>
@@ -6744,8 +8147,11 @@
       <c r="F188" t="s">
         <v>474</v>
       </c>
-    </row>
-    <row r="189" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I188" s="2" t="s">
+        <v>1028</v>
+      </c>
+    </row>
+    <row r="189" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
         <v>475</v>
       </c>
@@ -6764,8 +8170,11 @@
       <c r="F189" t="s">
         <v>476</v>
       </c>
-    </row>
-    <row r="190" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I189" s="2" t="s">
+        <v>1029</v>
+      </c>
+    </row>
+    <row r="190" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
         <v>477</v>
       </c>
@@ -6784,8 +8193,11 @@
       <c r="F190" t="s">
         <v>478</v>
       </c>
-    </row>
-    <row r="191" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I190" s="2" t="s">
+        <v>1030</v>
+      </c>
+    </row>
+    <row r="191" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
         <v>479</v>
       </c>
@@ -6805,7 +8217,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="192" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
         <v>481</v>
       </c>
@@ -6827,8 +8239,11 @@
       <c r="G192" t="s">
         <v>484</v>
       </c>
-    </row>
-    <row r="193" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I192" s="2" t="s">
+        <v>1031</v>
+      </c>
+    </row>
+    <row r="193" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
         <v>485</v>
       </c>
@@ -6847,8 +8262,11 @@
       <c r="F193" t="s">
         <v>486</v>
       </c>
-    </row>
-    <row r="194" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I193" s="2" t="s">
+        <v>1032</v>
+      </c>
+    </row>
+    <row r="194" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
         <v>487</v>
       </c>
@@ -6867,8 +8285,11 @@
       <c r="F194" t="s">
         <v>488</v>
       </c>
-    </row>
-    <row r="195" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I194" s="2" t="s">
+        <v>1033</v>
+      </c>
+    </row>
+    <row r="195" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
         <v>489</v>
       </c>
@@ -6887,8 +8308,11 @@
       <c r="F195" t="s">
         <v>490</v>
       </c>
-    </row>
-    <row r="196" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I195" s="2" t="s">
+        <v>1034</v>
+      </c>
+    </row>
+    <row r="196" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
         <v>491</v>
       </c>
@@ -6907,8 +8331,11 @@
       <c r="F196" t="s">
         <v>492</v>
       </c>
-    </row>
-    <row r="197" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I196" s="2" t="s">
+        <v>1035</v>
+      </c>
+    </row>
+    <row r="197" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
         <v>493</v>
       </c>
@@ -6927,8 +8354,11 @@
       <c r="F197" t="s">
         <v>494</v>
       </c>
-    </row>
-    <row r="198" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I197" s="2" t="s">
+        <v>1036</v>
+      </c>
+    </row>
+    <row r="198" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
         <v>495</v>
       </c>
@@ -6947,8 +8377,11 @@
       <c r="F198" t="s">
         <v>496</v>
       </c>
-    </row>
-    <row r="199" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I198" s="2" t="s">
+        <v>1037</v>
+      </c>
+    </row>
+    <row r="199" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
         <v>497</v>
       </c>
@@ -6967,8 +8400,11 @@
       <c r="F199" t="s">
         <v>498</v>
       </c>
-    </row>
-    <row r="200" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I199" s="2" t="s">
+        <v>1038</v>
+      </c>
+    </row>
+    <row r="200" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
         <v>499</v>
       </c>
@@ -6987,8 +8423,11 @@
       <c r="F200" t="s">
         <v>500</v>
       </c>
-    </row>
-    <row r="201" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I200" s="2" t="s">
+        <v>1039</v>
+      </c>
+    </row>
+    <row r="201" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
         <v>501</v>
       </c>
@@ -7007,8 +8446,11 @@
       <c r="F201" t="s">
         <v>502</v>
       </c>
-    </row>
-    <row r="202" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I201" s="2" t="s">
+        <v>1040</v>
+      </c>
+    </row>
+    <row r="202" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
         <v>503</v>
       </c>
@@ -7027,8 +8469,11 @@
       <c r="F202" t="s">
         <v>504</v>
       </c>
-    </row>
-    <row r="203" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I202" s="2" t="s">
+        <v>1041</v>
+      </c>
+    </row>
+    <row r="203" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
         <v>505</v>
       </c>
@@ -7047,8 +8492,11 @@
       <c r="F203" t="s">
         <v>506</v>
       </c>
-    </row>
-    <row r="204" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I203" s="2" t="s">
+        <v>1042</v>
+      </c>
+    </row>
+    <row r="204" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
         <v>507</v>
       </c>
@@ -7067,8 +8515,11 @@
       <c r="F204" t="s">
         <v>508</v>
       </c>
-    </row>
-    <row r="205" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I204" s="2" t="s">
+        <v>1043</v>
+      </c>
+    </row>
+    <row r="205" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
         <v>509</v>
       </c>
@@ -7087,8 +8538,11 @@
       <c r="F205" t="s">
         <v>510</v>
       </c>
-    </row>
-    <row r="206" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I205" s="2" t="s">
+        <v>1044</v>
+      </c>
+    </row>
+    <row r="206" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
         <v>511</v>
       </c>
@@ -7107,8 +8561,11 @@
       <c r="F206" t="s">
         <v>512</v>
       </c>
-    </row>
-    <row r="207" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I206" s="2" t="s">
+        <v>1045</v>
+      </c>
+    </row>
+    <row r="207" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
         <v>513</v>
       </c>
@@ -7127,8 +8584,11 @@
       <c r="F207" t="s">
         <v>514</v>
       </c>
-    </row>
-    <row r="208" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I207" s="2" t="s">
+        <v>1046</v>
+      </c>
+    </row>
+    <row r="208" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
         <v>515</v>
       </c>
@@ -7150,8 +8610,11 @@
       <c r="G208" t="s">
         <v>518</v>
       </c>
-    </row>
-    <row r="209" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I208" s="2" t="s">
+        <v>1047</v>
+      </c>
+    </row>
+    <row r="209" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
         <v>519</v>
       </c>
@@ -7173,8 +8636,11 @@
       <c r="G209" t="s">
         <v>522</v>
       </c>
-    </row>
-    <row r="210" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I209" s="2" t="s">
+        <v>1048</v>
+      </c>
+    </row>
+    <row r="210" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
         <v>523</v>
       </c>
@@ -7193,8 +8659,11 @@
       <c r="F210" t="s">
         <v>524</v>
       </c>
-    </row>
-    <row r="211" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I210" s="2" t="s">
+        <v>1049</v>
+      </c>
+    </row>
+    <row r="211" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
         <v>525</v>
       </c>
@@ -7213,8 +8682,11 @@
       <c r="F211" t="s">
         <v>526</v>
       </c>
-    </row>
-    <row r="212" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I211" s="2" t="s">
+        <v>1050</v>
+      </c>
+    </row>
+    <row r="212" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
         <v>527</v>
       </c>
@@ -7236,8 +8708,11 @@
       <c r="G212" t="s">
         <v>530</v>
       </c>
-    </row>
-    <row r="213" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I212" s="2" t="s">
+        <v>1051</v>
+      </c>
+    </row>
+    <row r="213" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
         <v>531</v>
       </c>
@@ -7256,8 +8731,11 @@
       <c r="F213" t="s">
         <v>532</v>
       </c>
-    </row>
-    <row r="214" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I213" s="2" t="s">
+        <v>1052</v>
+      </c>
+    </row>
+    <row r="214" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
         <v>533</v>
       </c>
@@ -7279,8 +8757,11 @@
       <c r="G214" t="s">
         <v>536</v>
       </c>
-    </row>
-    <row r="215" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I214" s="2" t="s">
+        <v>1053</v>
+      </c>
+    </row>
+    <row r="215" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
         <v>537</v>
       </c>
@@ -7299,8 +8780,11 @@
       <c r="F215" t="s">
         <v>538</v>
       </c>
-    </row>
-    <row r="216" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I215" s="2" t="s">
+        <v>1054</v>
+      </c>
+    </row>
+    <row r="216" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
         <v>539</v>
       </c>
@@ -7319,8 +8803,11 @@
       <c r="F216" t="s">
         <v>540</v>
       </c>
-    </row>
-    <row r="217" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I216" s="2" t="s">
+        <v>1055</v>
+      </c>
+    </row>
+    <row r="217" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
         <v>541</v>
       </c>
@@ -7342,8 +8829,11 @@
       <c r="G217" t="s">
         <v>544</v>
       </c>
-    </row>
-    <row r="218" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I217" s="2" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="218" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
         <v>545</v>
       </c>
@@ -7362,8 +8852,11 @@
       <c r="F218" t="s">
         <v>546</v>
       </c>
-    </row>
-    <row r="219" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I218" s="2" t="s">
+        <v>1057</v>
+      </c>
+    </row>
+    <row r="219" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
         <v>547</v>
       </c>
@@ -7382,8 +8875,11 @@
       <c r="F219" t="s">
         <v>548</v>
       </c>
-    </row>
-    <row r="220" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I219" s="2" t="s">
+        <v>1058</v>
+      </c>
+    </row>
+    <row r="220" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
         <v>549</v>
       </c>
@@ -7402,8 +8898,11 @@
       <c r="F220" t="s">
         <v>550</v>
       </c>
-    </row>
-    <row r="221" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I220" s="2" t="s">
+        <v>1059</v>
+      </c>
+    </row>
+    <row r="221" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
         <v>551</v>
       </c>
@@ -7422,8 +8921,11 @@
       <c r="F221" t="s">
         <v>552</v>
       </c>
-    </row>
-    <row r="222" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I221" s="2" t="s">
+        <v>1060</v>
+      </c>
+    </row>
+    <row r="222" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
         <v>553</v>
       </c>
@@ -7442,8 +8944,11 @@
       <c r="F222" t="s">
         <v>554</v>
       </c>
-    </row>
-    <row r="223" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I222" s="2" t="s">
+        <v>1061</v>
+      </c>
+    </row>
+    <row r="223" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
         <v>555</v>
       </c>
@@ -7462,8 +8967,11 @@
       <c r="F223" t="s">
         <v>556</v>
       </c>
-    </row>
-    <row r="224" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I223" s="2" t="s">
+        <v>1062</v>
+      </c>
+    </row>
+    <row r="224" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
         <v>557</v>
       </c>
@@ -7482,8 +8990,11 @@
       <c r="F224" t="s">
         <v>558</v>
       </c>
-    </row>
-    <row r="225" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I224" s="2" t="s">
+        <v>1063</v>
+      </c>
+    </row>
+    <row r="225" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
         <v>559</v>
       </c>
@@ -7502,8 +9013,11 @@
       <c r="F225" t="s">
         <v>560</v>
       </c>
-    </row>
-    <row r="226" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I225" s="2" t="s">
+        <v>1064</v>
+      </c>
+    </row>
+    <row r="226" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
         <v>561</v>
       </c>
@@ -7522,8 +9036,11 @@
       <c r="F226" t="s">
         <v>562</v>
       </c>
-    </row>
-    <row r="227" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I226" s="2" t="s">
+        <v>1065</v>
+      </c>
+    </row>
+    <row r="227" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
         <v>563</v>
       </c>
@@ -7542,8 +9059,11 @@
       <c r="F227" t="s">
         <v>564</v>
       </c>
-    </row>
-    <row r="228" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I227" s="2" t="s">
+        <v>1066</v>
+      </c>
+    </row>
+    <row r="228" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
         <v>565</v>
       </c>
@@ -7562,8 +9082,11 @@
       <c r="F228" t="s">
         <v>829</v>
       </c>
-    </row>
-    <row r="229" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I228" s="2" t="s">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="229" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
         <v>566</v>
       </c>
@@ -7582,8 +9105,11 @@
       <c r="F229" t="s">
         <v>567</v>
       </c>
-    </row>
-    <row r="230" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I229" s="2" t="s">
+        <v>1068</v>
+      </c>
+    </row>
+    <row r="230" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
         <v>568</v>
       </c>
@@ -7602,8 +9128,11 @@
       <c r="F230" t="s">
         <v>569</v>
       </c>
-    </row>
-    <row r="231" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I230" s="2" t="s">
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="231" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
         <v>570</v>
       </c>
@@ -7622,8 +9151,11 @@
       <c r="F231" t="s">
         <v>571</v>
       </c>
-    </row>
-    <row r="232" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I231" s="2" t="s">
+        <v>1070</v>
+      </c>
+    </row>
+    <row r="232" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
         <v>572</v>
       </c>
@@ -7642,8 +9174,11 @@
       <c r="F232" t="s">
         <v>573</v>
       </c>
-    </row>
-    <row r="233" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I232" s="2" t="s">
+        <v>1071</v>
+      </c>
+    </row>
+    <row r="233" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
         <v>574</v>
       </c>
@@ -7662,8 +9197,11 @@
       <c r="F233" t="s">
         <v>575</v>
       </c>
-    </row>
-    <row r="234" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I233" s="2" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="234" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
         <v>576</v>
       </c>
@@ -7682,8 +9220,11 @@
       <c r="F234" t="s">
         <v>577</v>
       </c>
-    </row>
-    <row r="235" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I234" s="2" t="s">
+        <v>1073</v>
+      </c>
+    </row>
+    <row r="235" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
         <v>578</v>
       </c>
@@ -7702,8 +9243,11 @@
       <c r="F235" t="s">
         <v>579</v>
       </c>
-    </row>
-    <row r="236" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I235" s="2" t="s">
+        <v>1074</v>
+      </c>
+    </row>
+    <row r="236" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
         <v>580</v>
       </c>
@@ -7722,8 +9266,11 @@
       <c r="F236" t="s">
         <v>581</v>
       </c>
-    </row>
-    <row r="237" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I236" s="2" t="s">
+        <v>1075</v>
+      </c>
+    </row>
+    <row r="237" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
         <v>582</v>
       </c>
@@ -7745,8 +9292,11 @@
       <c r="G237" t="s">
         <v>585</v>
       </c>
-    </row>
-    <row r="238" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I237" s="2" t="s">
+        <v>1076</v>
+      </c>
+    </row>
+    <row r="238" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
         <v>586</v>
       </c>
@@ -7765,8 +9315,11 @@
       <c r="F238" t="s">
         <v>587</v>
       </c>
-    </row>
-    <row r="239" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I238" s="2" t="s">
+        <v>1077</v>
+      </c>
+    </row>
+    <row r="239" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
         <v>588</v>
       </c>
@@ -7785,8 +9338,11 @@
       <c r="F239" t="s">
         <v>589</v>
       </c>
-    </row>
-    <row r="240" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I239" s="2" t="s">
+        <v>1078</v>
+      </c>
+    </row>
+    <row r="240" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A240" t="s">
         <v>590</v>
       </c>
@@ -7805,8 +9361,11 @@
       <c r="F240" t="s">
         <v>591</v>
       </c>
-    </row>
-    <row r="241" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I240" s="2" t="s">
+        <v>1079</v>
+      </c>
+    </row>
+    <row r="241" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
         <v>592</v>
       </c>
@@ -7825,8 +9384,11 @@
       <c r="F241" t="s">
         <v>593</v>
       </c>
-    </row>
-    <row r="242" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I241" s="2" t="s">
+        <v>1080</v>
+      </c>
+    </row>
+    <row r="242" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
         <v>594</v>
       </c>
@@ -7848,8 +9410,11 @@
       <c r="G242" t="s">
         <v>597</v>
       </c>
-    </row>
-    <row r="243" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I242" s="2" t="s">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="243" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
         <v>598</v>
       </c>
@@ -7868,8 +9433,11 @@
       <c r="F243" t="s">
         <v>599</v>
       </c>
-    </row>
-    <row r="244" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I243" s="2" t="s">
+        <v>1082</v>
+      </c>
+    </row>
+    <row r="244" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A244" t="s">
         <v>600</v>
       </c>
@@ -7888,8 +9456,11 @@
       <c r="F244" t="s">
         <v>601</v>
       </c>
-    </row>
-    <row r="245" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I244" s="2" t="s">
+        <v>1083</v>
+      </c>
+    </row>
+    <row r="245" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A245" t="s">
         <v>602</v>
       </c>
@@ -7908,8 +9479,11 @@
       <c r="F245" t="s">
         <v>603</v>
       </c>
-    </row>
-    <row r="246" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I245" s="2" t="s">
+        <v>1084</v>
+      </c>
+    </row>
+    <row r="246" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
         <v>604</v>
       </c>
@@ -7928,8 +9502,11 @@
       <c r="F246" t="s">
         <v>605</v>
       </c>
-    </row>
-    <row r="247" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I246" s="2" t="s">
+        <v>1085</v>
+      </c>
+    </row>
+    <row r="247" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A247" t="s">
         <v>606</v>
       </c>
@@ -7948,8 +9525,11 @@
       <c r="F247" t="s">
         <v>607</v>
       </c>
-    </row>
-    <row r="248" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I247" s="2" t="s">
+        <v>1086</v>
+      </c>
+    </row>
+    <row r="248" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A248" t="s">
         <v>608</v>
       </c>
@@ -7968,8 +9548,11 @@
       <c r="F248" t="s">
         <v>609</v>
       </c>
-    </row>
-    <row r="249" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I248" s="2" t="s">
+        <v>1087</v>
+      </c>
+    </row>
+    <row r="249" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A249" t="s">
         <v>610</v>
       </c>
@@ -7988,8 +9571,11 @@
       <c r="F249" t="s">
         <v>611</v>
       </c>
-    </row>
-    <row r="250" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I249" s="2" t="s">
+        <v>1088</v>
+      </c>
+    </row>
+    <row r="250" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A250" t="s">
         <v>612</v>
       </c>
@@ -8008,8 +9594,11 @@
       <c r="F250" t="s">
         <v>613</v>
       </c>
-    </row>
-    <row r="251" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I250" s="2" t="s">
+        <v>1089</v>
+      </c>
+    </row>
+    <row r="251" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A251" t="s">
         <v>614</v>
       </c>
@@ -8031,8 +9620,11 @@
       <c r="G251" t="s">
         <v>617</v>
       </c>
-    </row>
-    <row r="252" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I251" s="2" t="s">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="252" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A252" t="s">
         <v>618</v>
       </c>
@@ -8051,8 +9643,11 @@
       <c r="F252" t="s">
         <v>619</v>
       </c>
-    </row>
-    <row r="253" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I252" s="2" t="s">
+        <v>1091</v>
+      </c>
+    </row>
+    <row r="253" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A253" t="s">
         <v>620</v>
       </c>
@@ -8071,8 +9666,11 @@
       <c r="F253" t="s">
         <v>621</v>
       </c>
-    </row>
-    <row r="254" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I253" s="2" t="s">
+        <v>1092</v>
+      </c>
+    </row>
+    <row r="254" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A254" t="s">
         <v>622</v>
       </c>
@@ -8091,8 +9689,11 @@
       <c r="F254" t="s">
         <v>623</v>
       </c>
-    </row>
-    <row r="255" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I254" s="2" t="s">
+        <v>1093</v>
+      </c>
+    </row>
+    <row r="255" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A255" t="s">
         <v>624</v>
       </c>
@@ -8111,8 +9712,11 @@
       <c r="F255" t="s">
         <v>625</v>
       </c>
-    </row>
-    <row r="256" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I255" s="2" t="s">
+        <v>1094</v>
+      </c>
+    </row>
+    <row r="256" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A256" t="s">
         <v>626</v>
       </c>
@@ -8131,8 +9735,11 @@
       <c r="F256" t="s">
         <v>627</v>
       </c>
-    </row>
-    <row r="257" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I256" s="2" t="s">
+        <v>1095</v>
+      </c>
+    </row>
+    <row r="257" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A257" t="s">
         <v>628</v>
       </c>
@@ -8153,6 +9760,9 @@
       </c>
       <c r="G257" t="s">
         <v>631</v>
+      </c>
+      <c r="I257" s="2" t="s">
+        <v>1096</v>
       </c>
     </row>
   </sheetData>

</xml_diff>